<commit_message>
Actualizando documentacion - v.1.2
</commit_message>
<xml_diff>
--- a/Documentacion/Kanban.xlsx
+++ b/Documentacion/Kanban.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudia Ursula\Documents\Crodi Shop - Tienda online\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudia Ursula\Documents\Crodi Shop - Tienda online\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DDE593-764A-481C-976F-9F9B3BDE636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1F5A43-BBCF-458A-8CA0-03C3C475FFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{751C78DB-5605-4FC3-BE93-D922210FE98D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>To do</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Crea modelos para productos y usuarios en Django</t>
-  </si>
-  <si>
     <t>Implementa vistas y APIs básicas con Django REST Framework</t>
   </si>
   <si>
@@ -84,6 +81,21 @@
   </si>
   <si>
     <t>Ejecuta el servidor de desarrollo de React</t>
+  </si>
+  <si>
+    <t>Configurar la base de datos en Django</t>
+  </si>
+  <si>
+    <t>Crear el modelo de Usuario</t>
+  </si>
+  <si>
+    <t>Crear el modelo de Producto</t>
+  </si>
+  <si>
+    <t>Aplicar migraciones y verificar modelos en la base de datos</t>
+  </si>
+  <si>
+    <t>Registrar modelos en el panel de administración de Django</t>
   </si>
 </sst>
 </file>
@@ -298,6 +310,104 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <strike val="0"/>
@@ -329,104 +439,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -441,12 +453,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C14" totalsRowShown="0" headerRowDxfId="0" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:C14" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C19" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C19" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C45C42D6-BEBB-4324-8A88-0EBD89A37AAB}" name="To do" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{B7128B19-C3CB-4786-A9E8-41BC5FB7999B}" name="In Progress" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{CEAD33BE-683E-41EB-8288-E7FA6AEA13B1}" name="Done" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{C45C42D6-BEBB-4324-8A88-0EBD89A37AAB}" name="To do" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{B7128B19-C3CB-4786-A9E8-41BC5FB7999B}" name="In Progress" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{CEAD33BE-683E-41EB-8288-E7FA6AEA13B1}" name="Done" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -769,17 +781,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA60855-ABD8-405D-9BF4-3BBFB4305F47}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
@@ -797,92 +808,125 @@
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizando documentacion - v.1.3
</commit_message>
<xml_diff>
--- a/Documentacion/Kanban.xlsx
+++ b/Documentacion/Kanban.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudia Ursula\Documents\Crodi Shop - Tienda online\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1F5A43-BBCF-458A-8CA0-03C3C475FFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869F12F0-98C2-4637-B488-2D8F85B993C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{751C78DB-5605-4FC3-BE93-D922210FE98D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>To do</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Implementa vistas y APIs básicas con Django REST Framework</t>
-  </si>
-  <si>
     <t>Diseña el esquema inicial de la base de datos (SQLite/PostgreSQL)</t>
   </si>
   <si>
@@ -96,6 +93,21 @@
   </si>
   <si>
     <t>Registrar modelos en el panel de administración de Django</t>
+  </si>
+  <si>
+    <t>Instalar y configurar Django REST Framework</t>
+  </si>
+  <si>
+    <t>Crear serializadores para usuarios y productos</t>
+  </si>
+  <si>
+    <t>Implementar vistas basadas en API para usuarios y productos</t>
+  </si>
+  <si>
+    <t>Configurar las URLs para la API</t>
+  </si>
+  <si>
+    <t>Probar los endpoints en Postman o el navegador</t>
   </si>
 </sst>
 </file>
@@ -275,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -304,6 +316,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,8 +466,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C19" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C19" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C23" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C23" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C45C42D6-BEBB-4324-8A88-0EBD89A37AAB}" name="To do" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{B7128B19-C3CB-4786-A9E8-41BC5FB7999B}" name="In Progress" dataDxfId="1"/>
@@ -781,16 +794,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA60855-ABD8-405D-9BF4-3BBFB4305F47}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="50.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
@@ -808,125 +821,153 @@
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="5"/>
+      <c r="C16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-    </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizando documentacion - v.1.4
</commit_message>
<xml_diff>
--- a/Documentacion/Kanban.xlsx
+++ b/Documentacion/Kanban.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudia Ursula\Documents\Crodi Shop - Tienda online\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869F12F0-98C2-4637-B488-2D8F85B993C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172565EC-B7BD-4F14-A055-61FED25A0DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{751C78DB-5605-4FC3-BE93-D922210FE98D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>To do</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Diseña el esquema inicial de la base de datos (SQLite/PostgreSQL)</t>
-  </si>
-  <si>
     <t>Diseña una página básica con React y conecta al backend</t>
   </si>
   <si>
@@ -108,6 +105,18 @@
   </si>
   <si>
     <t>Probar los endpoints en Postman o el navegador</t>
+  </si>
+  <si>
+    <t>Definir el esquema de la base de datos</t>
+  </si>
+  <si>
+    <t>Crear las migraciones y aplicar cambios en la base de datos</t>
+  </si>
+  <si>
+    <t>Verificar el esquema en Django Admin y probarlo</t>
+  </si>
+  <si>
+    <t>Diseña el esquema inicial de la base de datos</t>
   </si>
 </sst>
 </file>
@@ -466,8 +475,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C23" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C23" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C26" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C26" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C45C42D6-BEBB-4324-8A88-0EBD89A37AAB}" name="To do" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{B7128B19-C3CB-4786-A9E8-41BC5FB7999B}" name="In Progress" dataDxfId="1"/>
@@ -794,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA60855-ABD8-405D-9BF4-3BBFB4305F47}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,153 +830,174 @@
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="5"/>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="2"/>
       <c r="C18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="10"/>
       <c r="C19" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
+      <c r="C23" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizando documentacion - v.1.5
</commit_message>
<xml_diff>
--- a/Documentacion/Kanban.xlsx
+++ b/Documentacion/Kanban.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudia Ursula\Documents\Crodi Shop - Tienda online\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172565EC-B7BD-4F14-A055-61FED25A0DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C6C708-1363-482B-8C96-0EAD2D94E8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{751C78DB-5605-4FC3-BE93-D922210FE98D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>To do</t>
   </si>
@@ -117,6 +117,21 @@
   </si>
   <si>
     <t>Diseña el esquema inicial de la base de datos</t>
+  </si>
+  <si>
+    <t>Configurar React y organizar la estructura del proyecto</t>
+  </si>
+  <si>
+    <t>Crear una página de inicio básica</t>
+  </si>
+  <si>
+    <t>Configurar CORS en Django para permitir conexiones desde React</t>
+  </si>
+  <si>
+    <t>Crear servicio para conectar con la API</t>
+  </si>
+  <si>
+    <t>Probar conexión entre React y Django</t>
   </si>
 </sst>
 </file>
@@ -173,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -281,22 +296,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -311,9 +315,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -475,8 +476,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C26" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C26" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C30" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C30" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C45C42D6-BEBB-4324-8A88-0EBD89A37AAB}" name="To do" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{B7128B19-C3CB-4786-A9E8-41BC5FB7999B}" name="In Progress" dataDxfId="1"/>
@@ -803,26 +804,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA60855-ABD8-405D-9BF4-3BBFB4305F47}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="55.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -947,7 +948,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
-      <c r="B19" s="10"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="5" t="s">
         <v>21</v>
       </c>
@@ -988,16 +989,46 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="4"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizando documentacion - v.2.1
</commit_message>
<xml_diff>
--- a/Documentacion/Kanban.xlsx
+++ b/Documentacion/Kanban.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudia Ursula\Documents\Crodi Shop - Tienda online\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C6C708-1363-482B-8C96-0EAD2D94E8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352FE255-E7A9-4B0E-BF4F-5CB2BB044182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{751C78DB-5605-4FC3-BE93-D922210FE98D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>To do</t>
   </si>
@@ -132,13 +132,76 @@
   </si>
   <si>
     <t>Probar conexión entre React y Django</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Crear el modelo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>Carrito</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>CarritoItem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> en Django</t>
+    </r>
+  </si>
+  <si>
+    <t>Crear las vistas del carrito con Django REST Framework</t>
+  </si>
+  <si>
+    <t>Crear los serializers para el carrito</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Configurar las rutas en </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>urls.py</t>
+    </r>
+  </si>
+  <si>
+    <t>Probar las APIs del carrito con Postman</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +223,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="5">
@@ -476,8 +544,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C30" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C30" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C35" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C35" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C45C42D6-BEBB-4324-8A88-0EBD89A37AAB}" name="To do" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{B7128B19-C3CB-4786-A9E8-41BC5FB7999B}" name="In Progress" dataDxfId="1"/>
@@ -804,19 +872,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA60855-ABD8-405D-9BF4-3BBFB4305F47}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="83" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="54.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="55.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -827,207 +895,242 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="1"/>
       <c r="B16" s="5"/>
       <c r="C16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" s="4"/>
       <c r="B18" s="2"/>
       <c r="C18" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" s="4"/>
       <c r="B19" s="9"/>
       <c r="C19" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="4"/>
       <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="1"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" s="4"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" s="4"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" s="4"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" s="4"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" s="4"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" s="4"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizando documentacion - v.2.2
</commit_message>
<xml_diff>
--- a/Documentacion/Kanban.xlsx
+++ b/Documentacion/Kanban.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudia Ursula\Documents\Crodi Shop - Tienda online\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352FE255-E7A9-4B0E-BF4F-5CB2BB044182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE446381-EB20-4B85-BE77-0A9ABC4D9BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{751C78DB-5605-4FC3-BE93-D922210FE98D}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{751C78DB-5605-4FC3-BE93-D922210FE98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>To do</t>
   </si>
@@ -195,6 +195,31 @@
   </si>
   <si>
     <t>Probar las APIs del carrito con Postman</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Crear el componente </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>Catalogo.js</t>
+    </r>
+  </si>
+  <si>
+    <t>Configurar las rutas en React Router</t>
+  </si>
+  <si>
+    <t>Agregar un enlace al catálogo en la barra de navegación</t>
+  </si>
+  <si>
+    <t>Agregar estilos con Bootstrap</t>
+  </si>
+  <si>
+    <t>Probar la página del catálogo en el navegador</t>
   </si>
 </sst>
 </file>
@@ -256,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -364,11 +389,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -395,6 +431,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,8 +583,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C35" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C35" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}" name="Tabla1" displayName="Tabla1" ref="A1:C40" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C40" xr:uid="{8C5935FF-C5BC-4A15-85C1-9F1D55DC885C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C45C42D6-BEBB-4324-8A88-0EBD89A37AAB}" name="To do" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{B7128B19-C3CB-4786-A9E8-41BC5FB7999B}" name="In Progress" dataDxfId="1"/>
@@ -872,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA60855-ABD8-405D-9BF4-3BBFB4305F47}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="83" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="83" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1133,6 +1172,41 @@
         <v>36</v>
       </c>
     </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="10"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="10"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>